<commit_message>
back lambda in main menu
</commit_message>
<xml_diff>
--- a/lesson.01/db/tel_book.xlsx
+++ b/lesson.01/db/tel_book.xlsx
@@ -1,123 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9660" windowWidth="16095" xWindow="240" yWindow="15"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>ФИО</t>
-  </si>
-  <si>
-    <t>Телефон</t>
-  </si>
-  <si>
-    <t>Комментарий</t>
-  </si>
-  <si>
-    <t>Дата добавления</t>
-  </si>
-  <si>
-    <t>Оптимус прайм</t>
-  </si>
-  <si>
-    <t>Робот полицейский</t>
-  </si>
-  <si>
-    <t>Юрий Гагарин</t>
-  </si>
-  <si>
-    <t>Александр</t>
-  </si>
-  <si>
-    <t>Александр Д.</t>
-  </si>
-  <si>
-    <t>Кот Вася</t>
-  </si>
-  <si>
-    <t>Александр Невский</t>
-  </si>
-  <si>
-    <t>Защитник</t>
-  </si>
-  <si>
-    <t>Всегда идет на помощь</t>
-  </si>
-  <si>
-    <t>Первый в космосе</t>
-  </si>
-  <si>
-    <t>Тест</t>
-  </si>
-  <si>
-    <t>Студент OTUS</t>
-  </si>
-  <si>
-    <t>Вернулся домой</t>
-  </si>
-  <si>
-    <t>Великий полководец</t>
-  </si>
-  <si>
-    <t>2024-08-21 22:09:44</t>
-  </si>
-  <si>
-    <t>2024-08-21 23:32:06</t>
-  </si>
-  <si>
-    <t>2024-08-22 00:35:15</t>
-  </si>
-  <si>
-    <t>2024-08-22 00:36:35</t>
-  </si>
-  <si>
-    <t>2024-08-22 14:20:40</t>
-  </si>
-  <si>
-    <t>2024-08-22 14:23:31</t>
-  </si>
-  <si>
-    <t>2024-08-22 18:15:21</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -148,19 +66,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -448,150 +365,258 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ФИО</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Телефон</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Комментарий</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Дата добавления</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Оптимус прайм</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>6969696</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Защитник</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2024-08-21 22:09:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Робот полицейский</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>6969696</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Всегда идет на помощь</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2024-08-21 23:32:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Юрий Гагарин</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>89015555555</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Первый в космосе</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2024-08-22 00:35:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>7</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Александр</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>89260010101</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Тест</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2024-08-22 00:36:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>8</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Александр Д.</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>89267263610</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Студент OTUS</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2024-08-22 14:20:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>9</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Кот Вася</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>911</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Вернулся домой</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2024-08-22 14:23:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>10</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Александр Невский</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>10000000001</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Великий полководец</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:15:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>11</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Кот Ляпольд</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2-22-22</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Давайте жить дружно</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2024-08-28 01:04:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>89015555555</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>89260010101</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>89267263610</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>911</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8">
-        <v>10000000001</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
-        <v>25</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Друг Кота</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>000</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Совсем маленький друг</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2024-08-28 01:08:21</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>